<commit_message>
compared RTP IDs between project list and layers in 2040
</commit_message>
<xml_diff>
--- a/projlist/Working DRAFT 2045 Project List.xlsx
+++ b/projlist/Working DRAFT 2045 Project List.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30112A7A-07D4-4FF8-B23A-04438919ACD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\GitHub\RTP\projlist\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17BDCA1-4098-412E-911D-BB1EF1488D4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="21" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="3210" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto Constrained - Arterial Lin" sheetId="2" r:id="rId1"/>
@@ -32,7 +37,7 @@
     <sheet name="Table Data" sheetId="26" r:id="rId22"/>
     <sheet name="Bike Illustrative onstreet wout" sheetId="21" r:id="rId23"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -48,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="1130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2859" uniqueCount="1130">
   <si>
     <t>Name</t>
   </si>
@@ -4098,7 +4103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4748,6 +4753,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4828,6 +4839,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5194,10 +5208,10 @@
       <c r="G1" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="217" t="s">
+      <c r="H1" s="219" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="218"/>
+      <c r="I1" s="220"/>
       <c r="J1" s="206" t="s">
         <v>8</v>
       </c>
@@ -5215,13 +5229,13 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="20.25">
-      <c r="A2" s="219" t="s">
+      <c r="A2" s="221" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
       <c r="F2" s="91"/>
       <c r="G2" s="86"/>
       <c r="H2" s="86"/>
@@ -5234,7 +5248,7 @@
       <c r="M2" s="76"/>
       <c r="N2" s="76"/>
     </row>
-    <row r="3" spans="1:14" ht="110.25">
+    <row r="3" spans="1:14" ht="106.5">
       <c r="A3" s="88" t="s">
         <v>15</v>
       </c>
@@ -5274,7 +5288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="63">
+    <row r="4" spans="1:14" ht="61.5">
       <c r="A4" s="77" t="s">
         <v>24</v>
       </c>
@@ -5311,7 +5325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="63">
+    <row r="5" spans="1:14" ht="61.5">
       <c r="A5" s="23" t="s">
         <v>24</v>
       </c>
@@ -5388,7 +5402,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:14" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -5410,10 +5424,10 @@
       <c r="G1" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>585</v>
       </c>
-      <c r="I1" s="229"/>
+      <c r="I1" s="231"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -5431,22 +5445,22 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="27" customHeight="1">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="230" t="s">
         <v>586</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
+      <c r="L2" s="230"/>
+      <c r="M2" s="230"/>
+      <c r="N2" s="230"/>
     </row>
     <row r="3" spans="1:14" ht="45">
       <c r="A3" s="1" t="s">
@@ -5488,7 +5502,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="75">
+    <row r="4" spans="1:14" ht="45">
       <c r="A4" s="1" t="s">
         <v>591</v>
       </c>
@@ -5608,7 +5622,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="135">
+    <row r="7" spans="1:14" ht="105">
       <c r="A7" s="77" t="s">
         <v>36</v>
       </c>
@@ -5648,7 +5662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="75">
+    <row r="8" spans="1:14" ht="60">
       <c r="A8" s="23" t="s">
         <v>610</v>
       </c>
@@ -5853,10 +5867,10 @@
       <c r="G1" s="211" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="230" t="s">
+      <c r="H1" s="232" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="231"/>
+      <c r="I1" s="233"/>
       <c r="J1" s="211" t="s">
         <v>8</v>
       </c>
@@ -5874,19 +5888,19 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="20.25">
-      <c r="A2" s="232" t="s">
+      <c r="A2" s="234" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
+      <c r="B2" s="234"/>
+      <c r="C2" s="234"/>
+      <c r="D2" s="234"/>
+      <c r="E2" s="234"/>
+      <c r="F2" s="234"/>
+      <c r="G2" s="234"/>
+      <c r="H2" s="234"/>
+      <c r="I2" s="234"/>
+      <c r="J2" s="234"/>
+      <c r="K2" s="234"/>
       <c r="L2" s="116"/>
       <c r="M2" s="116"/>
       <c r="N2" s="116"/>
@@ -6211,7 +6225,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="105">
+    <row r="1" spans="1:14" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -6233,10 +6247,10 @@
       <c r="G1" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -6254,22 +6268,22 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="230" t="s">
         <v>657</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
+      <c r="L2" s="230"/>
+      <c r="M2" s="230"/>
+      <c r="N2" s="230"/>
     </row>
     <row r="3" spans="1:14" ht="75">
       <c r="A3" s="1" t="s">
@@ -6398,7 +6412,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45">
+    <row r="1" spans="1:11" ht="60">
       <c r="A1" s="213" t="s">
         <v>0</v>
       </c>
@@ -6420,10 +6434,10 @@
       <c r="G1" s="213" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="234" t="s">
+      <c r="H1" s="236" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="234"/>
+      <c r="I1" s="236"/>
       <c r="J1" s="213" t="s">
         <v>8</v>
       </c>
@@ -6432,19 +6446,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="226" t="s">
         <v>672</v>
       </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="8" t="s">
@@ -6645,10 +6659,10 @@
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A9" s="235" t="s">
+      <c r="A9" s="237" t="s">
         <v>684</v>
       </c>
-      <c r="B9" s="235"/>
+      <c r="B9" s="237"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="45">
@@ -6966,10 +6980,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75">
-      <c r="A19" s="224" t="s">
+      <c r="A19" s="226" t="s">
         <v>689</v>
       </c>
-      <c r="B19" s="224"/>
+      <c r="B19" s="226"/>
     </row>
     <row r="20" spans="1:11" ht="90">
       <c r="A20" s="8" t="s">
@@ -7175,17 +7189,17 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="30" customHeight="1">
-      <c r="C27" s="233" t="s">
+      <c r="C27" s="235" t="s">
         <v>694</v>
       </c>
-      <c r="D27" s="233"/>
+      <c r="D27" s="235"/>
       <c r="F27" s="6">
         <f>SUM(F25+F18+F8)</f>
         <v>707325000</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6">
-        <f t="shared" ref="G27:I27" si="6">SUM(H25+H18+H8)</f>
+        <f t="shared" ref="H27:I27" si="6">SUM(H25+H18+H8)</f>
         <v>1044872422.9749932</v>
       </c>
       <c r="I27" s="6">
@@ -7228,7 +7242,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45">
+    <row r="1" spans="1:11" ht="60">
       <c r="A1" s="209" t="s">
         <v>0</v>
       </c>
@@ -7250,10 +7264,10 @@
       <c r="G1" s="209" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="225" t="s">
+      <c r="H1" s="227" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="225"/>
+      <c r="I1" s="227"/>
       <c r="J1" s="209" t="s">
         <v>8</v>
       </c>
@@ -7404,7 +7418,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="45">
+    <row r="1" spans="1:16" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -7426,10 +7440,10 @@
       <c r="G1" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -7447,22 +7461,22 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="18.75">
-      <c r="A2" s="236" t="s">
+      <c r="A2" s="238" t="s">
         <v>697</v>
       </c>
-      <c r="B2" s="236"/>
-      <c r="C2" s="236"/>
-      <c r="D2" s="236"/>
-      <c r="E2" s="236"/>
-      <c r="F2" s="236"/>
-      <c r="G2" s="236"/>
-      <c r="H2" s="236"/>
-      <c r="I2" s="236"/>
-      <c r="J2" s="236"/>
-      <c r="K2" s="236"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="236"/>
-      <c r="N2" s="236"/>
+      <c r="B2" s="238"/>
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="238"/>
+      <c r="F2" s="238"/>
+      <c r="G2" s="238"/>
+      <c r="H2" s="238"/>
+      <c r="I2" s="238"/>
+      <c r="J2" s="238"/>
+      <c r="K2" s="238"/>
+      <c r="L2" s="238"/>
+      <c r="M2" s="238"/>
+      <c r="N2" s="238"/>
     </row>
     <row r="3" spans="1:16" s="67" customFormat="1" ht="135">
       <c r="A3" s="214" t="s">
@@ -7506,7 +7520,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="105">
+    <row r="4" spans="1:16" ht="75">
       <c r="A4" s="1" t="s">
         <v>706</v>
       </c>
@@ -8257,7 +8271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="135">
+    <row r="22" spans="1:14" ht="75">
       <c r="A22" s="23" t="s">
         <v>786</v>
       </c>
@@ -8301,7 +8315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="135">
+    <row r="23" spans="1:14" ht="75">
       <c r="A23" s="23" t="s">
         <v>789</v>
       </c>
@@ -8389,7 +8403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="135">
+    <row r="25" spans="1:14" ht="75">
       <c r="A25" s="23" t="s">
         <v>796</v>
       </c>
@@ -8433,7 +8447,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="90">
+    <row r="26" spans="1:14" ht="60">
       <c r="A26" s="23" t="s">
         <v>799</v>
       </c>
@@ -8648,7 +8662,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="105">
+    <row r="1" spans="1:14" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -8670,10 +8684,10 @@
       <c r="G1" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -8691,24 +8705,24 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="45" customHeight="1">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="230" t="s">
         <v>822</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228"/>
-    </row>
-    <row r="3" spans="1:14" ht="165">
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
+      <c r="L2" s="230"/>
+      <c r="M2" s="230"/>
+      <c r="N2" s="230"/>
+    </row>
+    <row r="3" spans="1:14" ht="150">
       <c r="A3" s="1" t="s">
         <v>744</v>
       </c>
@@ -8814,10 +8828,10 @@
       <c r="G1" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -8835,22 +8849,22 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="230" t="s">
         <v>825</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
+      <c r="L2" s="230"/>
+      <c r="M2" s="230"/>
+      <c r="N2" s="230"/>
     </row>
     <row r="3" spans="1:15" ht="75">
       <c r="A3" s="214" t="s">
@@ -9249,7 +9263,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="51">
+    <row r="13" spans="1:15" ht="60">
       <c r="A13" s="77" t="s">
         <v>378</v>
       </c>
@@ -9289,7 +9303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="51">
+    <row r="14" spans="1:15" ht="60">
       <c r="A14" s="23" t="s">
         <v>387</v>
       </c>
@@ -9449,7 +9463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="75">
+    <row r="18" spans="1:15" ht="90">
       <c r="A18" s="23" t="s">
         <v>139</v>
       </c>
@@ -9748,7 +9762,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45">
+    <row r="1" spans="1:15" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -9770,10 +9784,10 @@
       <c r="G1" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -10675,7 +10689,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="60">
+    <row r="25" spans="1:14" ht="51">
       <c r="A25" s="48" t="s">
         <v>942</v>
       </c>
@@ -12309,7 +12323,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45">
+    <row r="1" spans="1:18" ht="60">
       <c r="A1" s="209" t="s">
         <v>0</v>
       </c>
@@ -12331,10 +12345,10 @@
       <c r="G1" s="209" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="225" t="s">
+      <c r="H1" s="227" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="225"/>
+      <c r="I1" s="227"/>
       <c r="J1" s="209" t="s">
         <v>8</v>
       </c>
@@ -12352,19 +12366,19 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="18.75">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="239" t="s">
         <v>697</v>
       </c>
-      <c r="B2" s="237"/>
-      <c r="C2" s="237"/>
-      <c r="D2" s="237"/>
-      <c r="E2" s="237"/>
-      <c r="F2" s="237"/>
-      <c r="G2" s="237"/>
-      <c r="H2" s="237"/>
-      <c r="I2" s="237"/>
-      <c r="J2" s="237"/>
-      <c r="K2" s="237"/>
+      <c r="B2" s="239"/>
+      <c r="C2" s="239"/>
+      <c r="D2" s="239"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="239"/>
+      <c r="I2" s="239"/>
+      <c r="J2" s="239"/>
+      <c r="K2" s="239"/>
     </row>
     <row r="3" spans="1:18" ht="105">
       <c r="A3" s="8" t="s">
@@ -12399,12 +12413,12 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="238" t="s">
+      <c r="O3" s="240" t="s">
         <v>1073</v>
       </c>
-      <c r="P3" s="238"/>
-      <c r="Q3" s="238"/>
-      <c r="R3" s="238"/>
+      <c r="P3" s="240"/>
+      <c r="Q3" s="240"/>
+      <c r="R3" s="240"/>
     </row>
     <row r="4" spans="1:18" ht="45">
       <c r="A4" s="23" t="s">
@@ -12445,10 +12459,10 @@
       <c r="N4" s="65" t="s">
         <v>1078</v>
       </c>
-      <c r="O4" s="238"/>
-      <c r="P4" s="238"/>
-      <c r="Q4" s="238"/>
-      <c r="R4" s="238"/>
+      <c r="O4" s="240"/>
+      <c r="P4" s="240"/>
+      <c r="Q4" s="240"/>
+      <c r="R4" s="240"/>
     </row>
     <row r="5" spans="1:18" ht="45">
       <c r="A5" s="23" t="s">
@@ -12489,10 +12503,10 @@
       <c r="N5" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="O5" s="238"/>
-      <c r="P5" s="238"/>
-      <c r="Q5" s="238"/>
-      <c r="R5" s="238"/>
+      <c r="O5" s="240"/>
+      <c r="P5" s="240"/>
+      <c r="Q5" s="240"/>
+      <c r="R5" s="240"/>
     </row>
     <row r="6" spans="1:18" ht="90">
       <c r="A6" s="23" t="s">
@@ -12533,10 +12547,10 @@
       <c r="N6" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="O6" s="238"/>
-      <c r="P6" s="238"/>
-      <c r="Q6" s="238"/>
-      <c r="R6" s="238"/>
+      <c r="O6" s="240"/>
+      <c r="P6" s="240"/>
+      <c r="Q6" s="240"/>
+      <c r="R6" s="240"/>
     </row>
     <row r="7" spans="1:18" ht="60">
       <c r="A7" s="1" t="s">
@@ -12696,7 +12710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="38.25">
+    <row r="12" spans="1:18" ht="39">
       <c r="A12" s="88" t="s">
         <v>1105</v>
       </c>
@@ -12918,10 +12932,10 @@
       <c r="G1" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="221" t="s">
+      <c r="H1" s="223" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="222"/>
+      <c r="I1" s="224"/>
       <c r="J1" s="71" t="s">
         <v>8</v>
       </c>
@@ -12939,24 +12953,24 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="20.25">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="225" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="223"/>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
-      <c r="J2" s="223"/>
-      <c r="K2" s="223"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
       <c r="L2" s="76"/>
       <c r="M2" s="76"/>
       <c r="N2" s="42"/>
     </row>
-    <row r="3" spans="1:14" ht="63">
+    <row r="3" spans="1:14" ht="61.5">
       <c r="A3" s="77" t="s">
         <v>36</v>
       </c>
@@ -13128,10 +13142,10 @@
       <c r="F1" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="217" t="s">
+      <c r="G1" s="219" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="218"/>
+      <c r="H1" s="220"/>
       <c r="I1" s="68" t="s">
         <v>8</v>
       </c>
@@ -13204,10 +13218,10 @@
       <c r="F1" s="215" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="240" t="s">
+      <c r="G1" s="242" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="241"/>
+      <c r="H1" s="243"/>
       <c r="I1" s="68" t="s">
         <v>8</v>
       </c>
@@ -13225,18 +13239,18 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="20.25">
-      <c r="A2" s="239" t="s">
+      <c r="A2" s="241" t="s">
         <v>825</v>
       </c>
-      <c r="B2" s="239"/>
-      <c r="C2" s="239"/>
-      <c r="D2" s="239"/>
-      <c r="E2" s="239"/>
-      <c r="F2" s="239"/>
-      <c r="G2" s="239"/>
-      <c r="H2" s="239"/>
-      <c r="I2" s="239"/>
-      <c r="J2" s="239"/>
+      <c r="B2" s="241"/>
+      <c r="C2" s="241"/>
+      <c r="D2" s="241"/>
+      <c r="E2" s="241"/>
+      <c r="F2" s="241"/>
+      <c r="G2" s="241"/>
+      <c r="H2" s="241"/>
+      <c r="I2" s="241"/>
+      <c r="J2" s="241"/>
       <c r="K2" s="116"/>
       <c r="L2" s="116"/>
       <c r="M2" s="116"/>
@@ -13377,7 +13391,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEFA431-46D9-4EAF-B146-C65B14FD122C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -13433,10 +13449,10 @@
       <c r="F1" s="216" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="242" t="s">
+      <c r="G1" s="244" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="243"/>
+      <c r="H1" s="245"/>
       <c r="I1" s="74" t="s">
         <v>8</v>
       </c>
@@ -13454,18 +13470,18 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="20.25">
-      <c r="A2" s="239" t="s">
+      <c r="A2" s="241" t="s">
         <v>865</v>
       </c>
-      <c r="B2" s="239"/>
-      <c r="C2" s="239"/>
-      <c r="D2" s="239"/>
-      <c r="E2" s="239"/>
-      <c r="F2" s="239"/>
-      <c r="G2" s="239"/>
-      <c r="H2" s="239"/>
-      <c r="I2" s="239"/>
-      <c r="J2" s="239"/>
+      <c r="B2" s="241"/>
+      <c r="C2" s="241"/>
+      <c r="D2" s="241"/>
+      <c r="E2" s="241"/>
+      <c r="F2" s="241"/>
+      <c r="G2" s="241"/>
+      <c r="H2" s="241"/>
+      <c r="I2" s="241"/>
+      <c r="J2" s="241"/>
       <c r="K2" s="116"/>
       <c r="L2" s="116"/>
       <c r="M2" s="116"/>
@@ -13552,7 +13568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="45">
+    <row r="5" spans="1:14" ht="60">
       <c r="A5" s="88" t="s">
         <v>1122</v>
       </c>
@@ -13676,7 +13692,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:14" ht="60">
       <c r="A1" s="209" t="s">
         <v>0</v>
       </c>
@@ -13698,10 +13714,10 @@
       <c r="G1" s="209" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="225" t="s">
+      <c r="H1" s="227" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="225"/>
+      <c r="I1" s="227"/>
       <c r="J1" s="209" t="s">
         <v>8</v>
       </c>
@@ -13719,11 +13735,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="226" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
     </row>
     <row r="3" spans="1:14" ht="45">
       <c r="A3" s="1" t="s">
@@ -13956,7 +13972,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="90">
+    <row r="9" spans="1:14" ht="60">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
@@ -14073,7 +14089,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="60">
+    <row r="12" spans="1:14" ht="45">
       <c r="A12" s="1" t="s">
         <v>100</v>
       </c>
@@ -14153,7 +14169,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="75">
+    <row r="14" spans="1:14" ht="60">
       <c r="A14" s="1" t="s">
         <v>70</v>
       </c>
@@ -14233,7 +14249,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="60">
+    <row r="16" spans="1:14" ht="45">
       <c r="A16" s="1" t="s">
         <v>117</v>
       </c>
@@ -14313,7 +14329,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="150">
+    <row r="18" spans="1:14" ht="120">
       <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
@@ -14353,7 +14369,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="60">
+    <row r="19" spans="1:14" ht="45">
       <c r="A19" s="1" t="s">
         <v>130</v>
       </c>
@@ -14640,7 +14656,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:14" ht="60">
       <c r="A1" s="209" t="s">
         <v>0</v>
       </c>
@@ -14662,10 +14678,10 @@
       <c r="G1" s="209" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="225" t="s">
+      <c r="H1" s="227" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="225"/>
+      <c r="I1" s="227"/>
       <c r="J1" s="209" t="s">
         <v>8</v>
       </c>
@@ -14683,11 +14699,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75">
-      <c r="A2" s="226" t="s">
+      <c r="A2" s="228" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="226"/>
+      <c r="B2" s="228"/>
+      <c r="C2" s="228"/>
     </row>
     <row r="3" spans="1:14" ht="45">
       <c r="A3" s="8" t="s">
@@ -15329,7 +15345,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="45">
+    <row r="19" spans="1:14" ht="30">
       <c r="A19" s="8" t="s">
         <v>236</v>
       </c>
@@ -15529,7 +15545,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="45">
+    <row r="24" spans="1:14" ht="30">
       <c r="A24" s="23" t="s">
         <v>257</v>
       </c>
@@ -15569,7 +15585,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="60">
+    <row r="25" spans="1:14" ht="30">
       <c r="A25" s="23" t="s">
         <v>263</v>
       </c>
@@ -15609,7 +15625,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="60">
+    <row r="26" spans="1:14" ht="30">
       <c r="A26" s="23" t="s">
         <v>266</v>
       </c>
@@ -15769,7 +15785,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="90">
+    <row r="30" spans="1:14" ht="105">
       <c r="A30" s="23" t="s">
         <v>280</v>
       </c>
@@ -15851,7 +15867,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45">
+    <row r="1" spans="1:15" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -15873,10 +15889,10 @@
       <c r="G1" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -15894,11 +15910,11 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="226" t="s">
         <v>285</v>
       </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
     </row>
     <row r="3" spans="1:15" ht="75">
       <c r="A3" s="8" t="s">
@@ -16101,7 +16117,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="105">
+    <row r="8" spans="1:15" ht="75">
       <c r="A8" s="8" t="s">
         <v>216</v>
       </c>
@@ -16141,7 +16157,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="105">
+    <row r="9" spans="1:15" ht="75">
       <c r="A9" s="8" t="s">
         <v>316</v>
       </c>
@@ -16181,7 +16197,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="105">
+    <row r="10" spans="1:15" ht="75">
       <c r="A10" s="8" t="s">
         <v>319</v>
       </c>
@@ -16221,7 +16237,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="120">
+    <row r="11" spans="1:15" ht="90">
       <c r="A11" s="8" t="s">
         <v>322</v>
       </c>
@@ -16261,7 +16277,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="105">
+    <row r="12" spans="1:15" ht="75">
       <c r="A12" s="8" t="s">
         <v>135</v>
       </c>
@@ -16341,7 +16357,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="105">
+    <row r="14" spans="1:15" ht="90">
       <c r="A14" s="8" t="s">
         <v>240</v>
       </c>
@@ -16381,7 +16397,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="150">
+    <row r="15" spans="1:15" ht="105">
       <c r="A15" s="8" t="s">
         <v>338</v>
       </c>
@@ -16501,7 +16517,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="105">
+    <row r="18" spans="1:14" ht="75">
       <c r="A18" s="8" t="s">
         <v>352</v>
       </c>
@@ -16541,7 +16557,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="105">
+    <row r="19" spans="1:14" ht="75">
       <c r="A19" s="8" t="s">
         <v>247</v>
       </c>
@@ -16661,7 +16677,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="120">
+    <row r="22" spans="1:14" ht="90">
       <c r="A22" s="8" t="s">
         <v>370</v>
       </c>
@@ -16701,7 +16717,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="105">
+    <row r="23" spans="1:14" ht="75">
       <c r="A23" s="8" t="s">
         <v>204</v>
       </c>
@@ -16739,7 +16755,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="120">
+    <row r="24" spans="1:14" ht="105">
       <c r="A24" s="23" t="s">
         <v>378</v>
       </c>
@@ -16779,7 +16795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="105">
+    <row r="25" spans="1:14" ht="120">
       <c r="A25" s="23" t="s">
         <v>382</v>
       </c>
@@ -17297,7 +17313,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17342,10 +17358,10 @@
       <c r="G1" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -17361,23 +17377,23 @@
       <c r="O1" s="210"/>
     </row>
     <row r="2" spans="1:15" ht="15.75">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="226" t="s">
         <v>435</v>
       </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
-      <c r="L2" s="224"/>
-      <c r="M2" s="224"/>
-      <c r="N2" s="224"/>
-      <c r="O2" s="224"/>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="226"/>
+      <c r="J2" s="226"/>
+      <c r="K2" s="226"/>
+      <c r="L2" s="226"/>
+      <c r="M2" s="226"/>
+      <c r="N2" s="226"/>
+      <c r="O2" s="226"/>
     </row>
     <row r="3" spans="1:15" ht="63">
       <c r="A3" s="142" t="s">
@@ -18187,7 +18203,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="185" customFormat="1" ht="90">
+    <row r="26" spans="1:14" s="185" customFormat="1" ht="90.75">
       <c r="A26" s="187" t="s">
         <v>533</v>
       </c>
@@ -18668,10 +18684,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18685,12 +18701,12 @@
     <col min="7" max="8" width="16.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="12" width="35" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="35" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45">
+    <row r="1" spans="1:13" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -18712,21 +18728,24 @@
       <c r="G1" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="210" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="210" t="s">
+      <c r="L1" s="217" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="210" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:13" ht="15.75">
       <c r="A2" s="208" t="s">
         <v>554</v>
       </c>
@@ -18740,9 +18759,10 @@
       <c r="I2" s="210"/>
       <c r="J2" s="210"/>
       <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-    </row>
-    <row r="3" spans="1:12" s="184" customFormat="1" ht="75">
+      <c r="L2" s="217"/>
+      <c r="M2" s="210"/>
+    </row>
+    <row r="3" spans="1:13" s="184" customFormat="1" ht="75">
       <c r="A3" s="214" t="s">
         <v>555</v>
       </c>
@@ -18772,11 +18792,12 @@
       </c>
       <c r="J3" s="214"/>
       <c r="K3" s="214"/>
-      <c r="L3" s="214" t="s">
+      <c r="L3" s="218"/>
+      <c r="M3" s="214" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="75">
+    <row r="4" spans="1:13" ht="75">
       <c r="A4" s="77" t="s">
         <v>560</v>
       </c>
@@ -18806,8 +18827,9 @@
       <c r="K4" s="79" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="105">
+      <c r="L4" s="76"/>
+    </row>
+    <row r="5" spans="1:13" ht="105">
       <c r="A5" s="194" t="s">
         <v>562</v>
       </c>
@@ -18835,7 +18857,8 @@
       <c r="K5" s="195" t="s">
         <v>565</v>
       </c>
-      <c r="L5" s="197"/>
+      <c r="L5" s="246"/>
+      <c r="M5" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18850,7 +18873,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18894,10 +18917,10 @@
       <c r="G1" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -18971,7 +18994,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:14" ht="60">
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
@@ -18993,10 +19016,10 @@
       <c r="G1" s="210" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="227" t="s">
+      <c r="H1" s="229" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="227"/>
+      <c r="I1" s="229"/>
       <c r="J1" s="210" t="s">
         <v>8</v>
       </c>
@@ -19014,22 +19037,22 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="230" t="s">
         <v>568</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
-      <c r="L2" s="228"/>
-      <c r="M2" s="228"/>
-      <c r="N2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
+      <c r="L2" s="230"/>
+      <c r="M2" s="230"/>
+      <c r="N2" s="230"/>
     </row>
     <row r="3" spans="1:14" ht="60">
       <c r="A3" s="35" t="s">
@@ -19111,7 +19134,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="75">
+    <row r="5" spans="1:14" ht="60">
       <c r="A5" s="36" t="s">
         <v>576</v>
       </c>

</xml_diff>